<commit_message>
Added save to file max,min,agv methods
</commit_message>
<xml_diff>
--- a/funcionarios.xlsx
+++ b/funcionarios.xlsx
@@ -209,13 +209,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.71"/>
@@ -460,6 +460,12 @@
         <v>30050</v>
       </c>
     </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D15" s="0" t="n">
+        <f aca="false">D13/11</f>
+        <v>2731.81818181818</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>